<commit_message>
Add 5 references to manuscript body.
</commit_message>
<xml_diff>
--- a/Figures/Table 1.xlsx
+++ b/Figures/Table 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/robert_e_clark_wsu_edu/Documents/Henry-Buck-Trail-Experiment/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_F25DC773A252ABDACC104889F958553C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{775E42B0-EE6B-4AA2-891C-4870FB748792}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="11_F25DC773A252ABDACC104889F958553C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFD6F997-7491-42AF-8A04-F61021FC5015}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -253,22 +253,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,22 +636,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F26"/>
+  <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.44140625" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -577,298 +664,320 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="6">
+      <c r="D3" s="7"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="4">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="D4" s="8"/>
+      <c r="E4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="4">
         <v>117</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="D5" s="8"/>
+      <c r="E5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="4">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="6">
+      <c r="D6" s="8"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="4">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="D7" s="8"/>
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="4">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="6">
+      <c r="D8" s="8"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="6">
+      <c r="D9" s="8"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="4">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6">
+      <c r="D10" s="8"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="D11" s="8"/>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="D12" s="8"/>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="4">
         <v>104</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="6">
+      <c r="D13" s="8"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="D15" s="8"/>
+      <c r="E15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="4">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="6">
+      <c r="D16" s="8"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4">
         <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="D17" s="8"/>
+      <c r="E17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="4">
         <v>115</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="6">
+      <c r="D18" s="8"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="D19" s="8"/>
+      <c r="E19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="4">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="6">
+      <c r="D20" s="8"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="4">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="6">
+      <c r="D21" s="8"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4">
         <v>89</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="6">
+      <c r="D22" s="8"/>
+      <c r="E22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="4">
         <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="6">
+      <c r="D23" s="8"/>
+      <c r="E23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="4">
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="6">
+      <c r="D24" s="9"/>
+      <c r="E24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="4">
         <v>253</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update citations and species list for ant-dispersed plant paper.
</commit_message>
<xml_diff>
--- a/Figures/Table 1.xlsx
+++ b/Figures/Table 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R Projects\Henry-Buck-Trail-Experiment\Figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/robert_e_clark_wsu_edu/Documents/Henry-Buck-Trail-Experiment/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0427DDD1-F354-480B-84B4-78E41B5841A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{0427DDD1-F354-480B-84B4-78E41B5841A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50EED285-47D5-4AA1-9BDD-7EB67FF9EB05}"/>
   <bookViews>
-    <workbookView xWindow="9458" yWindow="758" windowWidth="17610" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Native species" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
   <si>
     <t xml:space="preserve">Species </t>
   </si>
@@ -61,9 +61,6 @@
     <t>Trillium undulatum</t>
   </si>
   <si>
-    <t>Trilium cernuum</t>
-  </si>
-  <si>
     <t>Corydalis sempervirens</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Claytonia virginica</t>
   </si>
   <si>
-    <t>Claytonia caroliniana</t>
-  </si>
-  <si>
     <t>Uvularia grandiflora</t>
   </si>
   <si>
@@ -254,9 +248,6 @@
   </si>
   <si>
     <t>Oberrath &amp; Bohning-Gaese, 2002?</t>
-  </si>
-  <si>
-    <t>Peters et al, 2003</t>
   </si>
   <si>
     <t>Greater celandine</t>
@@ -285,30 +276,9 @@
     </r>
   </si>
   <si>
-    <t>*not in the main text citations yet</t>
-  </si>
-  <si>
-    <t>Smith et al. 1989*</t>
-  </si>
-  <si>
-    <t>Ruhren and Dudash 1996*</t>
-  </si>
-  <si>
-    <t>Gibson 1993*</t>
-  </si>
-  <si>
-    <t>Gunther and Lanza 1989*</t>
-  </si>
-  <si>
-    <t>Gates 1942*</t>
-  </si>
-  <si>
     <t>Plant species</t>
   </si>
   <si>
-    <t>Beattie and Culver 1981*</t>
-  </si>
-  <si>
     <t>Blunt-lobed hepatica</t>
   </si>
   <si>
@@ -318,33 +288,184 @@
     <t>Ant-dispersal reported</t>
   </si>
   <si>
-    <t>Anemone americana*</t>
+    <t>Anemone quinquefolia</t>
+  </si>
+  <si>
+    <t>Beattie and Culver 1981</t>
+  </si>
+  <si>
+    <t>Handel et al. 1981</t>
+  </si>
+  <si>
+    <t>Smith et al. 1989</t>
+  </si>
+  <si>
+    <t>Galium circaezans</t>
+  </si>
+  <si>
+    <t>Forest licorice</t>
+  </si>
+  <si>
+    <t>Gaddy 1986</t>
+  </si>
+  <si>
+    <t>Heithaus 1981</t>
+  </si>
+  <si>
+    <t>Ruhren and Dudash 1996</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">* Former synonym with </t>
+      <t>Anemone americana</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Claytonia caroliniana</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Former synonym with</t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>Hepatica nobilis</t>
+      <t xml:space="preserve"> Hepatica nobilis</t>
     </r>
   </si>
   <si>
-    <t>Anemone quinquefolia</t>
+    <t>Miller and Chambers 2006</t>
+  </si>
+  <si>
+    <t>Gunther and Lanza 1989</t>
+  </si>
+  <si>
+    <t>Plants that I could find no direct observations or tests of myrmecochory</t>
+  </si>
+  <si>
+    <t>Bellemare et al. 2002</t>
+  </si>
+  <si>
+    <t>Describes genus as ant-dispersed</t>
+  </si>
+  <si>
+    <t>Gibson 1993</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Elaiosome traits reported for relatives in this genus</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Trilium cernuum</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Robertson 1897</t>
+  </si>
+  <si>
+    <t>add v papilionicae</t>
+  </si>
+  <si>
+    <t>v pedata</t>
+  </si>
+  <si>
+    <t>viola eriocarpa</t>
+  </si>
+  <si>
+    <t>from beattie and lyons 1975</t>
+  </si>
+  <si>
+    <t>Bossard 1990</t>
+  </si>
+  <si>
+    <t>Tracing of ant-dispersed seeds: a new technique is about scotch broom</t>
+  </si>
+  <si>
+    <t>check out list from Mitchell et al. 2002, especially foamflower</t>
+  </si>
+  <si>
+    <t>Peters et al, 2003, Oberatth and boning gaese 2002</t>
+  </si>
+  <si>
+    <t>Pemberton and Irving: elaiosomes on weed seeds and the potential for myrmecochory in naturalist plants looks cool on this topic!</t>
+  </si>
+  <si>
+    <t>Thompson 1981</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +524,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -686,7 +827,6 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -766,6 +906,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1047,604 +1190,671 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.46484375" customWidth="1"/>
-    <col min="4" max="4" width="20.796875" customWidth="1"/>
-    <col min="5" max="5" width="27.06640625" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="12"/>
-      <c r="C2" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="34" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="11"/>
+      <c r="C2" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="G2" s="18"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="15">
+      <c r="B3" s="11"/>
+      <c r="C3" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="14">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="15">
+      <c r="B4" s="11"/>
+      <c r="C4" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="14">
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="15">
+      <c r="D5" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="14">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="15">
+      <c r="B6" s="11"/>
+      <c r="C6" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="14">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="15">
+      <c r="B7" s="11"/>
+      <c r="C7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="14">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="15">
+      <c r="B8" s="11"/>
+      <c r="C8" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="14">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="15">
+      <c r="D9" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="14">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="15">
+      <c r="D10" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="14">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="15">
+      <c r="B11" s="11"/>
+      <c r="C11" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="14">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="15">
+      <c r="B12" s="11"/>
+      <c r="C12" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="14">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E13" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="24" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D14" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="15">
+      <c r="B15" s="11"/>
+      <c r="C15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="14">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="15">
+      <c r="B16" s="11"/>
+      <c r="C16" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="14">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="23" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="15">
+      <c r="D17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="14">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="23" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="15">
+      <c r="D18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="14">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="23" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="15">
+      <c r="D19" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="14">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="15">
+      <c r="B20" s="11"/>
+      <c r="C20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="14">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="15">
+      <c r="B21" s="11"/>
+      <c r="C21" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="14">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B22" s="11"/>
+      <c r="C22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="15">
+      <c r="B23" s="11"/>
+      <c r="C23" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="14">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="27" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="26"/>
+      <c r="F24" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="15">
+      <c r="G24" s="18"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="14">
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B25" s="11"/>
+      <c r="C25" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="26"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B26" s="11"/>
+      <c r="C26" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="15">
+      <c r="B27" s="11"/>
+      <c r="C27" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="14">
         <v>253</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="19" t="s">
+      <c r="B28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="18"/>
+      <c r="C30" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B29" s="12"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="19"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C33" s="1"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="18"/>
+      <c r="C31" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="24"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:G25">
@@ -1657,24 +1867,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF583C5-C943-4DF5-A211-8933C7BAD37A}">
-  <dimension ref="A2:G16"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.46484375" customWidth="1"/>
-    <col min="4" max="4" width="35.73046875" customWidth="1"/>
-    <col min="5" max="5" width="30.9296875" customWidth="1"/>
-    <col min="6" max="6" width="31.3984375" customWidth="1"/>
-    <col min="7" max="7" width="39.19921875" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" customWidth="1"/>
+    <col min="7" max="7" width="39.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1683,170 +1893,181 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="4">
+      <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="4">
+      <c r="C4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>74</v>
+      <c r="C5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C6" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C7" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>61</v>
+      <c r="C8" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C9" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C10" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>57</v>
+      <c r="C11" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C12" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>62</v>
+      <c r="C13" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>64</v>
+      <c r="C14" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C15" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Table 1, update references.
</commit_message>
<xml_diff>
--- a/Figures/Table 1.xlsx
+++ b/Figures/Table 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/robert_e_clark_wsu_edu/Documents/Henry-Buck-Trail-Experiment/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{0427DDD1-F354-480B-84B4-78E41B5841A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50EED285-47D5-4AA1-9BDD-7EB67FF9EB05}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{0427DDD1-F354-480B-84B4-78E41B5841A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B807A131-CE08-45CD-8798-73BFF96A3D51}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Native species" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="117">
   <si>
     <t xml:space="preserve">Species </t>
   </si>
@@ -163,19 +163,10 @@
     <t>State Herbaria (2017)</t>
   </si>
   <si>
-    <t>Viola rotundifolia</t>
-  </si>
-  <si>
     <t>Round-leaved violet</t>
   </si>
   <si>
     <t>Literature claiming ant-dispersal</t>
-  </si>
-  <si>
-    <t>Viola striata</t>
-  </si>
-  <si>
-    <t>Striped cream violet</t>
   </si>
   <si>
     <t>Viola blanda</t>
@@ -459,6 +450,33 @@
   </si>
   <si>
     <t>Thompson 1981</t>
+  </si>
+  <si>
+    <t>Culver and Beattie 1978</t>
+  </si>
+  <si>
+    <t>Viola pedata</t>
+  </si>
+  <si>
+    <t>Birdfood violet</t>
+  </si>
+  <si>
+    <t>Viola rostrata</t>
+  </si>
+  <si>
+    <t>Long-spurred violet</t>
+  </si>
+  <si>
+    <t>Viola palmata</t>
+  </si>
+  <si>
+    <t>Wood violet</t>
+  </si>
+  <si>
+    <t>Beattie and Lyons 1975</t>
+  </si>
+  <si>
+    <t>Viola rotundifolia2</t>
   </si>
 </sst>
 </file>
@@ -559,7 +577,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -821,11 +839,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -909,6 +938,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,13 +1249,13 @@
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="11"/>
       <c r="C2" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>2</v>
@@ -1240,13 +1272,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="18"/>
@@ -1261,13 +1293,13 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>38</v>
@@ -1290,7 +1322,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>38</v>
@@ -1307,13 +1339,13 @@
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="18"/>
@@ -1334,7 +1366,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>38</v>
@@ -1357,7 +1389,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="18"/>
@@ -1378,7 +1410,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>38</v>
@@ -1401,7 +1433,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>38</v>
@@ -1424,7 +1456,7 @@
         <v>26</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>38</v>
@@ -1441,13 +1473,13 @@
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="18"/>
@@ -1468,7 +1500,7 @@
         <v>40</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>38</v>
@@ -1483,13 +1515,13 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="18"/>
@@ -1508,7 +1540,7 @@
         <v>28</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>38</v>
@@ -1519,19 +1551,23 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="22" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
+        <v>30</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="18"/>
       <c r="H16" s="11"/>
       <c r="I16" s="14">
@@ -1544,17 +1580,15 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>38</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F17" s="24"/>
       <c r="G17" s="18"/>
       <c r="H17" s="11"/>
       <c r="I17" s="14">
@@ -1567,15 +1601,17 @@
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="24"/>
+        <v>90</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="G18" s="18"/>
       <c r="H18" s="11"/>
       <c r="I18" s="14">
@@ -1588,17 +1624,15 @@
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="22" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>38</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F19" s="24"/>
       <c r="G19" s="18"/>
       <c r="H19" s="11"/>
       <c r="I19" s="14">
@@ -1611,13 +1645,13 @@
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F20" s="24"/>
       <c r="G20" s="18"/>
@@ -1632,13 +1666,13 @@
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="22" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="18"/>
@@ -1653,12 +1687,14 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="22" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>115</v>
+      </c>
       <c r="F22" s="24"/>
       <c r="G22" s="18"/>
       <c r="H22" s="11"/>
@@ -1669,16 +1705,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="11"/>
-      <c r="C23" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24" t="s">
-        <v>38</v>
-      </c>
+      <c r="C23" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="29"/>
       <c r="G23" s="18"/>
       <c r="H23" s="11"/>
       <c r="I23" s="14">
@@ -1691,15 +1727,15 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="28" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="29" t="s">
-        <v>38</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="29"/>
       <c r="G24" s="18"/>
       <c r="H24" s="11"/>
       <c r="I24" s="14">
@@ -1711,14 +1747,18 @@
         <v>23</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="25" t="s">
-        <v>42</v>
+      <c r="C25" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>38</v>
+      </c>
       <c r="G25" s="18"/>
       <c r="H25" s="11"/>
       <c r="I25" s="13"/>
@@ -1728,14 +1768,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="11"/>
-      <c r="C26" s="25" t="s">
-        <v>45</v>
+      <c r="C26" s="28" t="s">
+        <v>111</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="27"/>
+        <v>112</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" s="29"/>
       <c r="G26" s="18"/>
       <c r="H26" s="11"/>
       <c r="I26" s="13"/>
@@ -1751,7 +1793,9 @@
       <c r="D27" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="17"/>
+      <c r="E27" s="36" t="s">
+        <v>108</v>
+      </c>
       <c r="F27" s="15" t="s">
         <v>38</v>
       </c>
@@ -1766,6 +1810,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="11"/>
+      <c r="C28" s="8"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
@@ -1781,7 +1826,7 @@
     <row r="30" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B30" s="18"/>
       <c r="C30" s="35" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -1790,7 +1835,7 @@
     <row r="31" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B31" s="18"/>
       <c r="C31" s="35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -1804,7 +1849,7 @@
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
@@ -1825,35 +1870,57 @@
         <v>24</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F35" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C37" s="22" t="s">
         <v>96</v>
       </c>
+      <c r="D37" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" s="24"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1884,7 +1951,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1893,7 +1960,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -1907,13 +1974,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="3">
@@ -1925,7 +1992,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>27</v>
@@ -1941,13 +2008,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1955,7 +2022,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1963,7 +2030,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1971,10 +2038,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1982,7 +2049,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1990,7 +2057,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1998,13 +2065,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2012,7 +2079,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2020,10 +2087,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2031,16 +2098,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2048,7 +2115,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2056,18 +2123,18 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>